<commit_message>
Fixes to formatting removing commas for BNVP
Just a format update so Vensim can read the .csv
</commit_message>
<xml_diff>
--- a/InputData/trans/BNVP/BAU New Vehicle Price.xlsx
+++ b/InputData/trans/BNVP/BAU New Vehicle Price.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\murielle.gagnebin\Nextcloud\EPS_Transport\Murielle\BNVP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\European Union\Models\eps-eu\InputData\trans\BNVP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67F453DA-1533-4A3B-BB4D-A298432BA2E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C60E464C-BACC-4F0C-9735-E1BF9A5D690C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="11" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -43,12 +43,15 @@
     <definedName name="cpi_2019to2012">About!$A$139</definedName>
     <definedName name="cpi_2020to2012">About!$A$140</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -2043,8 +2046,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="7">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="167" formatCode="0.000"/>
@@ -2249,12 +2252,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyProtection="0">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2296,7 +2299,6 @@
     <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="4" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="9" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="5" xfId="10" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -2323,20 +2325,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="168" fontId="0" fillId="4" borderId="5" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="Body: normal cell" xfId="4" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Comma" xfId="10" builtinId="3"/>
+    <cellStyle name="Currency" xfId="8" builtinId="4"/>
     <cellStyle name="Font: Calibri, 9pt regular" xfId="6" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Footnotes: top row" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Header: bottom row" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Komma" xfId="10" builtinId="3"/>
-    <cellStyle name="Link" xfId="9" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
     <cellStyle name="Parent row" xfId="3" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 2" xfId="11" xr:uid="{E67DE464-DFF7-4D04-9A48-2CE80637E87F}"/>
     <cellStyle name="Table title" xfId="7" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="Währung" xfId="8" builtinId="4"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2456,7 +2460,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2778,9 +2782,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B148"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="56.28515625" customWidth="1"/>
   </cols>
@@ -2814,7 +2818,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="25" t="s">
         <v>597</v>
       </c>
     </row>
@@ -2842,7 +2846,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="25" t="s">
         <v>600</v>
       </c>
     </row>
@@ -2852,7 +2856,7 @@
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B16" s="40">
+      <c r="B16" s="39">
         <v>2018</v>
       </c>
     </row>
@@ -2875,7 +2879,7 @@
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="40">
+      <c r="B21" s="39">
         <v>2016</v>
       </c>
     </row>
@@ -3064,7 +3068,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="63" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:2" ht="45" x14ac:dyDescent="0.25">
       <c r="B63" s="20" t="s">
         <v>579</v>
       </c>
@@ -3487,7 +3491,7 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.42578125" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
@@ -4644,7 +4648,7 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.42578125" customWidth="1"/>
   </cols>
@@ -5731,7 +5735,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.42578125" customWidth="1"/>
     <col min="2" max="35" width="10" customWidth="1"/>
@@ -6747,7 +6751,7 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.42578125" customWidth="1"/>
     <col min="2" max="35" width="10.140625" customWidth="1"/>
@@ -7763,7 +7767,7 @@
       <selection activeCell="C2" sqref="C2:C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.42578125" customWidth="1"/>
   </cols>
@@ -8777,7 +8781,7 @@
       <selection activeCell="C2" sqref="C2:C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.42578125" customWidth="1"/>
   </cols>
@@ -9789,7 +9793,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.42578125" customWidth="1"/>
   </cols>
@@ -10702,7 +10706,7 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.42578125" customWidth="1"/>
   </cols>
@@ -11713,11 +11717,11 @@
   </sheetPr>
   <dimension ref="A1:AJ8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.42578125" customWidth="1"/>
     <col min="2" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
@@ -12117,139 +12121,139 @@
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="25">
+      <c r="B4" s="43">
         <f>Motorbikes!B5</f>
         <v>9937.9583061357698</v>
       </c>
-      <c r="C4" s="25">
+      <c r="C4" s="43">
         <f>Motorbikes!C5</f>
         <v>9651.84</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="43">
         <f>Motorbikes!D5</f>
         <v>9482.880000000001</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="43">
         <f>Motorbikes!E5</f>
         <v>9402.0640000000003</v>
       </c>
-      <c r="F4" s="23">
+      <c r="F4" s="44">
         <f>$E4</f>
         <v>9402.0640000000003</v>
       </c>
-      <c r="G4" s="23">
+      <c r="G4" s="44">
         <f t="shared" ref="G4:AI4" si="0">$E4</f>
         <v>9402.0640000000003</v>
       </c>
-      <c r="H4" s="23">
+      <c r="H4" s="44">
         <f t="shared" si="0"/>
         <v>9402.0640000000003</v>
       </c>
-      <c r="I4" s="23">
+      <c r="I4" s="44">
         <f t="shared" si="0"/>
         <v>9402.0640000000003</v>
       </c>
-      <c r="J4" s="23">
+      <c r="J4" s="44">
         <f t="shared" si="0"/>
         <v>9402.0640000000003</v>
       </c>
-      <c r="K4" s="23">
+      <c r="K4" s="44">
         <f t="shared" si="0"/>
         <v>9402.0640000000003</v>
       </c>
-      <c r="L4" s="23">
+      <c r="L4" s="44">
         <f t="shared" si="0"/>
         <v>9402.0640000000003</v>
       </c>
-      <c r="M4" s="23">
+      <c r="M4" s="44">
         <f t="shared" si="0"/>
         <v>9402.0640000000003</v>
       </c>
-      <c r="N4" s="23">
+      <c r="N4" s="44">
         <f t="shared" si="0"/>
         <v>9402.0640000000003</v>
       </c>
-      <c r="O4" s="23">
+      <c r="O4" s="44">
         <f t="shared" si="0"/>
         <v>9402.0640000000003</v>
       </c>
-      <c r="P4" s="23">
+      <c r="P4" s="44">
         <f t="shared" si="0"/>
         <v>9402.0640000000003</v>
       </c>
-      <c r="Q4" s="23">
+      <c r="Q4" s="44">
         <f t="shared" si="0"/>
         <v>9402.0640000000003</v>
       </c>
-      <c r="R4" s="23">
+      <c r="R4" s="44">
         <f t="shared" si="0"/>
         <v>9402.0640000000003</v>
       </c>
-      <c r="S4" s="23">
+      <c r="S4" s="44">
         <f t="shared" si="0"/>
         <v>9402.0640000000003</v>
       </c>
-      <c r="T4" s="23">
+      <c r="T4" s="44">
         <f t="shared" si="0"/>
         <v>9402.0640000000003</v>
       </c>
-      <c r="U4" s="23">
+      <c r="U4" s="44">
         <f t="shared" si="0"/>
         <v>9402.0640000000003</v>
       </c>
-      <c r="V4" s="23">
+      <c r="V4" s="44">
         <f t="shared" si="0"/>
         <v>9402.0640000000003</v>
       </c>
-      <c r="W4" s="23">
+      <c r="W4" s="44">
         <f t="shared" si="0"/>
         <v>9402.0640000000003</v>
       </c>
-      <c r="X4" s="23">
+      <c r="X4" s="44">
         <f t="shared" si="0"/>
         <v>9402.0640000000003</v>
       </c>
-      <c r="Y4" s="23">
+      <c r="Y4" s="44">
         <f t="shared" si="0"/>
         <v>9402.0640000000003</v>
       </c>
-      <c r="Z4" s="23">
+      <c r="Z4" s="44">
         <f t="shared" si="0"/>
         <v>9402.0640000000003</v>
       </c>
-      <c r="AA4" s="23">
+      <c r="AA4" s="44">
         <f t="shared" si="0"/>
         <v>9402.0640000000003</v>
       </c>
-      <c r="AB4" s="23">
+      <c r="AB4" s="44">
         <f t="shared" si="0"/>
         <v>9402.0640000000003</v>
       </c>
-      <c r="AC4" s="23">
+      <c r="AC4" s="44">
         <f t="shared" si="0"/>
         <v>9402.0640000000003</v>
       </c>
-      <c r="AD4" s="23">
+      <c r="AD4" s="44">
         <f t="shared" si="0"/>
         <v>9402.0640000000003</v>
       </c>
-      <c r="AE4" s="23">
+      <c r="AE4" s="44">
         <f t="shared" si="0"/>
         <v>9402.0640000000003</v>
       </c>
-      <c r="AF4" s="23">
+      <c r="AF4" s="44">
         <f t="shared" si="0"/>
         <v>9402.0640000000003</v>
       </c>
-      <c r="AG4" s="23">
+      <c r="AG4" s="44">
         <f t="shared" si="0"/>
         <v>9402.0640000000003</v>
       </c>
-      <c r="AH4" s="23">
+      <c r="AH4" s="44">
         <f t="shared" si="0"/>
         <v>9402.0640000000003</v>
       </c>
-      <c r="AI4" s="23">
+      <c r="AI4" s="44">
         <f t="shared" si="0"/>
         <v>9402.0640000000003</v>
       </c>
@@ -12698,7 +12702,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.42578125" customWidth="1"/>
   </cols>
@@ -13608,1191 +13612,1191 @@
       <selection activeCell="C9" sqref="C9:C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="28" t="s">
         <v>593</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="26" t="s">
         <v>599</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="26" t="s">
         <v>607</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="28">
+      <c r="B2" s="27">
         <v>23500</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="38">
+      <c r="C2" s="27"/>
+      <c r="D2" s="37">
         <f>B2*About!$A$145</f>
         <v>28620.854384948496</v>
       </c>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="26" t="s">
         <v>562</v>
       </c>
-      <c r="B3" s="28">
+      <c r="B3" s="27">
         <v>34500</v>
       </c>
-      <c r="C3" s="28"/>
-      <c r="D3" s="38">
+      <c r="C3" s="27"/>
+      <c r="D3" s="37">
         <f>B3*About!$A$145</f>
         <v>42017.850054498856</v>
       </c>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="26" t="s">
         <v>594</v>
       </c>
-      <c r="B4" s="28">
+      <c r="B4" s="27">
         <v>35400</v>
       </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="38">
+      <c r="C4" s="27"/>
+      <c r="D4" s="37">
         <f>B4*About!$A$145</f>
         <v>43113.967882007521</v>
       </c>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="26" t="s">
         <v>611</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28">
+      <c r="B5" s="27"/>
+      <c r="C5" s="27">
         <v>45835</v>
       </c>
-      <c r="D5" s="38">
+      <c r="D5" s="37">
         <f>C5*About!A146</f>
         <v>54178.399285986576</v>
       </c>
     </row>
-    <row r="8" spans="1:36" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
+    <row r="8" spans="1:36" s="32" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="30" t="s">
         <v>608</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="31" t="s">
         <v>609</v>
       </c>
-      <c r="C8" s="31">
+      <c r="C8" s="30">
         <v>2017</v>
       </c>
-      <c r="D8" s="31">
+      <c r="D8" s="30">
         <v>2018</v>
       </c>
-      <c r="E8" s="31">
+      <c r="E8" s="30">
         <v>2019</v>
       </c>
-      <c r="F8" s="31">
+      <c r="F8" s="30">
         <v>2020</v>
       </c>
-      <c r="G8" s="31">
+      <c r="G8" s="30">
         <v>2021</v>
       </c>
-      <c r="H8" s="31">
+      <c r="H8" s="30">
         <v>2022</v>
       </c>
-      <c r="I8" s="31">
+      <c r="I8" s="30">
         <v>2023</v>
       </c>
-      <c r="J8" s="31">
+      <c r="J8" s="30">
         <v>2024</v>
       </c>
-      <c r="K8" s="31">
+      <c r="K8" s="30">
         <v>2025</v>
       </c>
-      <c r="L8" s="31">
+      <c r="L8" s="30">
         <v>2026</v>
       </c>
-      <c r="M8" s="31">
+      <c r="M8" s="30">
         <v>2027</v>
       </c>
-      <c r="N8" s="31">
+      <c r="N8" s="30">
         <v>2028</v>
       </c>
-      <c r="O8" s="31">
+      <c r="O8" s="30">
         <v>2029</v>
       </c>
-      <c r="P8" s="31">
+      <c r="P8" s="30">
         <v>2030</v>
       </c>
-      <c r="Q8" s="31">
+      <c r="Q8" s="30">
         <v>2031</v>
       </c>
-      <c r="R8" s="31">
+      <c r="R8" s="30">
         <v>2032</v>
       </c>
-      <c r="S8" s="31">
+      <c r="S8" s="30">
         <v>2033</v>
       </c>
-      <c r="T8" s="31">
+      <c r="T8" s="30">
         <v>2034</v>
       </c>
-      <c r="U8" s="31">
+      <c r="U8" s="30">
         <v>2035</v>
       </c>
-      <c r="V8" s="31">
+      <c r="V8" s="30">
         <v>2036</v>
       </c>
-      <c r="W8" s="31">
+      <c r="W8" s="30">
         <v>2037</v>
       </c>
-      <c r="X8" s="31">
+      <c r="X8" s="30">
         <v>2038</v>
       </c>
-      <c r="Y8" s="31">
+      <c r="Y8" s="30">
         <v>2039</v>
       </c>
-      <c r="Z8" s="31">
+      <c r="Z8" s="30">
         <v>2040</v>
       </c>
-      <c r="AA8" s="31">
+      <c r="AA8" s="30">
         <v>2041</v>
       </c>
-      <c r="AB8" s="31">
+      <c r="AB8" s="30">
         <v>2042</v>
       </c>
-      <c r="AC8" s="31">
+      <c r="AC8" s="30">
         <v>2043</v>
       </c>
-      <c r="AD8" s="31">
+      <c r="AD8" s="30">
         <v>2044</v>
       </c>
-      <c r="AE8" s="31">
+      <c r="AE8" s="30">
         <v>2045</v>
       </c>
-      <c r="AF8" s="31">
+      <c r="AF8" s="30">
         <v>2046</v>
       </c>
-      <c r="AG8" s="31">
+      <c r="AG8" s="30">
         <v>2047</v>
       </c>
-      <c r="AH8" s="31">
+      <c r="AH8" s="30">
         <v>2048</v>
       </c>
-      <c r="AI8" s="31">
+      <c r="AI8" s="30">
         <v>2049</v>
       </c>
-      <c r="AJ8" s="31">
+      <c r="AJ8" s="30">
         <v>2050</v>
       </c>
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="37">
+      <c r="B9" s="36">
         <v>-5.0000000000000002E-5</v>
       </c>
-      <c r="C9" s="36">
+      <c r="C9" s="35">
         <f>D2</f>
         <v>28620.854384948496</v>
       </c>
-      <c r="D9" s="35">
+      <c r="D9" s="34">
         <f t="shared" ref="D9:AJ9" si="0">C9/(1-$B9)</f>
         <v>28619.423413777804</v>
       </c>
-      <c r="E9" s="35">
+      <c r="E9" s="34">
         <f t="shared" si="0"/>
         <v>28617.992514152094</v>
       </c>
-      <c r="F9" s="35">
+      <c r="F9" s="34">
         <f t="shared" si="0"/>
         <v>28616.561686067787</v>
       </c>
-      <c r="G9" s="35">
+      <c r="G9" s="34">
         <f t="shared" si="0"/>
         <v>28615.130929521307</v>
       </c>
-      <c r="H9" s="35">
+      <c r="H9" s="34">
         <f t="shared" si="0"/>
         <v>28613.700244509077</v>
       </c>
-      <c r="I9" s="35">
+      <c r="I9" s="34">
         <f t="shared" si="0"/>
         <v>28612.269631027521</v>
       </c>
-      <c r="J9" s="35">
+      <c r="J9" s="34">
         <f t="shared" si="0"/>
         <v>28610.839089073062</v>
       </c>
-      <c r="K9" s="35">
+      <c r="K9" s="34">
         <f t="shared" si="0"/>
         <v>28609.408618642126</v>
       </c>
-      <c r="L9" s="35">
+      <c r="L9" s="34">
         <f t="shared" si="0"/>
         <v>28607.978219731136</v>
       </c>
-      <c r="M9" s="35">
+      <c r="M9" s="34">
         <f t="shared" si="0"/>
         <v>28606.547892336515</v>
       </c>
-      <c r="N9" s="35">
+      <c r="N9" s="34">
         <f t="shared" si="0"/>
         <v>28605.117636454688</v>
       </c>
-      <c r="O9" s="35">
+      <c r="O9" s="34">
         <f t="shared" si="0"/>
         <v>28603.687452082082</v>
       </c>
-      <c r="P9" s="35">
+      <c r="P9" s="34">
         <f t="shared" si="0"/>
         <v>28602.257339215117</v>
       </c>
-      <c r="Q9" s="35">
+      <c r="Q9" s="34">
         <f t="shared" si="0"/>
         <v>28600.827297850221</v>
       </c>
-      <c r="R9" s="35">
+      <c r="R9" s="34">
         <f t="shared" si="0"/>
         <v>28599.397327983817</v>
       </c>
-      <c r="S9" s="35">
+      <c r="S9" s="34">
         <f t="shared" si="0"/>
         <v>28597.967429612334</v>
       </c>
-      <c r="T9" s="35">
+      <c r="T9" s="34">
         <f t="shared" si="0"/>
         <v>28596.537602732195</v>
       </c>
-      <c r="U9" s="35">
+      <c r="U9" s="34">
         <f t="shared" si="0"/>
         <v>28595.107847339823</v>
       </c>
-      <c r="V9" s="35">
+      <c r="V9" s="34">
         <f t="shared" si="0"/>
         <v>28593.678163431647</v>
       </c>
-      <c r="W9" s="35">
+      <c r="W9" s="34">
         <f t="shared" si="0"/>
         <v>28592.248551004093</v>
       </c>
-      <c r="X9" s="35">
+      <c r="X9" s="34">
         <f t="shared" si="0"/>
         <v>28590.819010053587</v>
       </c>
-      <c r="Y9" s="35">
+      <c r="Y9" s="34">
         <f t="shared" si="0"/>
         <v>28589.389540576554</v>
       </c>
-      <c r="Z9" s="35">
+      <c r="Z9" s="34">
         <f t="shared" si="0"/>
         <v>28587.960142569424</v>
       </c>
-      <c r="AA9" s="35">
+      <c r="AA9" s="34">
         <f t="shared" si="0"/>
         <v>28586.530816028619</v>
       </c>
-      <c r="AB9" s="35">
+      <c r="AB9" s="34">
         <f t="shared" si="0"/>
         <v>28585.101560950567</v>
       </c>
-      <c r="AC9" s="35">
+      <c r="AC9" s="34">
         <f t="shared" si="0"/>
         <v>28583.672377331695</v>
       </c>
-      <c r="AD9" s="35">
+      <c r="AD9" s="34">
         <f t="shared" si="0"/>
         <v>28582.243265168432</v>
       </c>
-      <c r="AE9" s="35">
+      <c r="AE9" s="34">
         <f t="shared" si="0"/>
         <v>28580.814224457205</v>
       </c>
-      <c r="AF9" s="35">
+      <c r="AF9" s="34">
         <f t="shared" si="0"/>
         <v>28579.38525519444</v>
       </c>
-      <c r="AG9" s="35">
+      <c r="AG9" s="34">
         <f t="shared" si="0"/>
         <v>28577.95635737657</v>
       </c>
-      <c r="AH9" s="35">
+      <c r="AH9" s="34">
         <f t="shared" si="0"/>
         <v>28576.527531000018</v>
       </c>
-      <c r="AI9" s="35">
+      <c r="AI9" s="34">
         <f t="shared" si="0"/>
         <v>28575.098776061212</v>
       </c>
-      <c r="AJ9" s="35">
+      <c r="AJ9" s="34">
         <f t="shared" si="0"/>
         <v>28573.670092556582</v>
       </c>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="26" t="s">
         <v>562</v>
       </c>
-      <c r="B10" s="37">
+      <c r="B10" s="36">
         <v>-5.0000000000000002E-5</v>
       </c>
-      <c r="C10" s="36">
+      <c r="C10" s="35">
         <f>D3</f>
         <v>42017.850054498856</v>
       </c>
-      <c r="D10" s="35">
+      <c r="D10" s="34">
         <f t="shared" ref="D10:AJ10" si="1">C10/(1-$B10)</f>
         <v>42015.749267035499</v>
       </c>
-      <c r="E10" s="35">
+      <c r="E10" s="34">
         <f t="shared" si="1"/>
         <v>42013.648584606264</v>
       </c>
-      <c r="F10" s="35">
+      <c r="F10" s="34">
         <f t="shared" si="1"/>
         <v>42011.5480072059</v>
       </c>
-      <c r="G10" s="35">
+      <c r="G10" s="34">
         <f t="shared" si="1"/>
         <v>42009.447534829153</v>
       </c>
-      <c r="H10" s="35">
+      <c r="H10" s="34">
         <f t="shared" si="1"/>
         <v>42007.347167470776</v>
       </c>
-      <c r="I10" s="35">
+      <c r="I10" s="34">
         <f t="shared" si="1"/>
         <v>42005.246905125518</v>
       </c>
-      <c r="J10" s="35">
+      <c r="J10" s="34">
         <f t="shared" si="1"/>
         <v>42003.146747788123</v>
       </c>
-      <c r="K10" s="35">
+      <c r="K10" s="34">
         <f t="shared" si="1"/>
         <v>42001.046695453348</v>
       </c>
-      <c r="L10" s="35">
+      <c r="L10" s="34">
         <f t="shared" si="1"/>
         <v>41998.946748115937</v>
       </c>
-      <c r="M10" s="35">
+      <c r="M10" s="34">
         <f t="shared" si="1"/>
         <v>41996.846905770646</v>
       </c>
-      <c r="N10" s="35">
+      <c r="N10" s="34">
         <f t="shared" si="1"/>
         <v>41994.747168412221</v>
       </c>
-      <c r="O10" s="35">
+      <c r="O10" s="34">
         <f t="shared" si="1"/>
         <v>41992.647536035416</v>
       </c>
-      <c r="P10" s="35">
+      <c r="P10" s="34">
         <f t="shared" si="1"/>
         <v>41990.548008634978</v>
       </c>
-      <c r="Q10" s="35">
+      <c r="Q10" s="34">
         <f t="shared" si="1"/>
         <v>41988.448586205661</v>
       </c>
-      <c r="R10" s="35">
+      <c r="R10" s="34">
         <f t="shared" si="1"/>
         <v>41986.349268742219</v>
       </c>
-      <c r="S10" s="35">
+      <c r="S10" s="34">
         <f t="shared" si="1"/>
         <v>41984.250056239405</v>
       </c>
-      <c r="T10" s="35">
+      <c r="T10" s="34">
         <f t="shared" si="1"/>
         <v>41982.150948691968</v>
       </c>
-      <c r="U10" s="35">
+      <c r="U10" s="34">
         <f t="shared" si="1"/>
         <v>41980.05194609466</v>
       </c>
-      <c r="V10" s="35">
+      <c r="V10" s="34">
         <f t="shared" si="1"/>
         <v>41977.953048442236</v>
       </c>
-      <c r="W10" s="35">
+      <c r="W10" s="34">
         <f t="shared" si="1"/>
         <v>41975.854255729442</v>
       </c>
-      <c r="X10" s="35">
+      <c r="X10" s="34">
         <f t="shared" si="1"/>
         <v>41973.755567951041</v>
       </c>
-      <c r="Y10" s="35">
+      <c r="Y10" s="34">
         <f t="shared" si="1"/>
         <v>41971.656985101778</v>
       </c>
-      <c r="Z10" s="35">
+      <c r="Z10" s="34">
         <f t="shared" si="1"/>
         <v>41969.558507176414</v>
       </c>
-      <c r="AA10" s="35">
+      <c r="AA10" s="34">
         <f t="shared" si="1"/>
         <v>41967.460134169698</v>
       </c>
-      <c r="AB10" s="35">
+      <c r="AB10" s="34">
         <f t="shared" si="1"/>
         <v>41965.36186607639</v>
       </c>
-      <c r="AC10" s="35">
+      <c r="AC10" s="34">
         <f t="shared" si="1"/>
         <v>41963.263702891243</v>
       </c>
-      <c r="AD10" s="35">
+      <c r="AD10" s="34">
         <f t="shared" si="1"/>
         <v>41961.165644609006</v>
       </c>
-      <c r="AE10" s="35">
+      <c r="AE10" s="34">
         <f t="shared" si="1"/>
         <v>41959.067691224438</v>
       </c>
-      <c r="AF10" s="35">
+      <c r="AF10" s="34">
         <f t="shared" si="1"/>
         <v>41956.969842732295</v>
       </c>
-      <c r="AG10" s="35">
+      <c r="AG10" s="34">
         <f t="shared" si="1"/>
         <v>41954.872099127337</v>
       </c>
-      <c r="AH10" s="35">
+      <c r="AH10" s="34">
         <f t="shared" si="1"/>
         <v>41952.774460404311</v>
       </c>
-      <c r="AI10" s="35">
+      <c r="AI10" s="34">
         <f t="shared" si="1"/>
         <v>41950.676926557979</v>
       </c>
-      <c r="AJ10" s="35">
+      <c r="AJ10" s="34">
         <f t="shared" si="1"/>
         <v>41948.579497583094</v>
       </c>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="26" t="s">
         <v>594</v>
       </c>
-      <c r="B11" s="37">
+      <c r="B11" s="36">
         <v>-5.0000000000000002E-5</v>
       </c>
-      <c r="C11" s="36">
+      <c r="C11" s="35">
         <f>D4</f>
         <v>43113.967882007521</v>
       </c>
-      <c r="D11" s="35">
+      <c r="D11" s="34">
         <f t="shared" ref="D11:AJ11" si="2">C11/(1-$B11)</f>
         <v>43111.812291392947</v>
       </c>
-      <c r="E11" s="35">
+      <c r="E11" s="34">
         <f t="shared" si="2"/>
         <v>43109.656808552514</v>
       </c>
-      <c r="F11" s="35">
+      <c r="F11" s="34">
         <f>E11/(1-$B11)</f>
         <v>43107.501433480837</v>
       </c>
-      <c r="G11" s="35">
+      <c r="G11" s="34">
         <f t="shared" si="2"/>
         <v>43105.346166172523</v>
       </c>
-      <c r="H11" s="35">
+      <c r="H11" s="34">
         <f t="shared" si="2"/>
         <v>43103.19100662219</v>
       </c>
-      <c r="I11" s="35">
+      <c r="I11" s="34">
         <f t="shared" si="2"/>
         <v>43101.035954824445</v>
       </c>
-      <c r="J11" s="35">
+      <c r="J11" s="34">
         <f t="shared" si="2"/>
         <v>43098.881010773905</v>
       </c>
-      <c r="K11" s="35">
+      <c r="K11" s="34">
         <f t="shared" si="2"/>
         <v>43096.726174465177</v>
       </c>
-      <c r="L11" s="35">
+      <c r="L11" s="34">
         <f t="shared" si="2"/>
         <v>43094.571445892878</v>
       </c>
-      <c r="M11" s="35">
+      <c r="M11" s="34">
         <f t="shared" si="2"/>
         <v>43092.416825051623</v>
       </c>
-      <c r="N11" s="35">
+      <c r="N11" s="34">
         <f t="shared" si="2"/>
         <v>43090.262311936021</v>
       </c>
-      <c r="O11" s="35">
+      <c r="O11" s="34">
         <f t="shared" si="2"/>
         <v>43088.107906540688</v>
       </c>
-      <c r="P11" s="35">
+      <c r="P11" s="34">
         <f t="shared" si="2"/>
         <v>43085.95360886024</v>
       </c>
-      <c r="Q11" s="35">
+      <c r="Q11" s="34">
         <f t="shared" si="2"/>
         <v>43083.799418889292</v>
       </c>
-      <c r="R11" s="35">
+      <c r="R11" s="34">
         <f t="shared" si="2"/>
         <v>43081.64533662246</v>
       </c>
-      <c r="S11" s="35">
+      <c r="S11" s="34">
         <f t="shared" si="2"/>
         <v>43079.491362054352</v>
       </c>
-      <c r="T11" s="35">
+      <c r="T11" s="34">
         <f t="shared" si="2"/>
         <v>43077.337495179585</v>
       </c>
-      <c r="U11" s="35">
+      <c r="U11" s="34">
         <f t="shared" si="2"/>
         <v>43075.183735992781</v>
       </c>
-      <c r="V11" s="35">
+      <c r="V11" s="34">
         <f t="shared" si="2"/>
         <v>43073.03008448855</v>
       </c>
-      <c r="W11" s="35">
+      <c r="W11" s="34">
         <f t="shared" si="2"/>
         <v>43070.876540661513</v>
       </c>
-      <c r="X11" s="35">
+      <c r="X11" s="34">
         <f t="shared" si="2"/>
         <v>43068.72310450628</v>
       </c>
-      <c r="Y11" s="35">
+      <c r="Y11" s="34">
         <f t="shared" si="2"/>
         <v>43066.569776017473</v>
       </c>
-      <c r="Z11" s="35">
+      <c r="Z11" s="34">
         <f t="shared" si="2"/>
         <v>43064.416555189709</v>
       </c>
-      <c r="AA11" s="35">
+      <c r="AA11" s="34">
         <f t="shared" si="2"/>
         <v>43062.263442017604</v>
       </c>
-      <c r="AB11" s="35">
+      <c r="AB11" s="34">
         <f t="shared" si="2"/>
         <v>43060.110436495772</v>
       </c>
-      <c r="AC11" s="35">
+      <c r="AC11" s="34">
         <f t="shared" si="2"/>
         <v>43057.957538618837</v>
       </c>
-      <c r="AD11" s="35">
+      <c r="AD11" s="34">
         <f t="shared" si="2"/>
         <v>43055.804748381415</v>
       </c>
-      <c r="AE11" s="35">
+      <c r="AE11" s="34">
         <f t="shared" si="2"/>
         <v>43053.652065778122</v>
       </c>
-      <c r="AF11" s="35">
+      <c r="AF11" s="34">
         <f t="shared" si="2"/>
         <v>43051.499490803581</v>
       </c>
-      <c r="AG11" s="35">
+      <c r="AG11" s="34">
         <f t="shared" si="2"/>
         <v>43049.347023452407</v>
       </c>
-      <c r="AH11" s="35">
+      <c r="AH11" s="34">
         <f t="shared" si="2"/>
         <v>43047.194663719216</v>
       </c>
-      <c r="AI11" s="35">
+      <c r="AI11" s="34">
         <f t="shared" si="2"/>
         <v>43045.042411598632</v>
       </c>
-      <c r="AJ11" s="35">
+      <c r="AJ11" s="34">
         <f t="shared" si="2"/>
         <v>43042.890267085269</v>
       </c>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="26" t="s">
         <v>610</v>
       </c>
-      <c r="B12" s="34">
+      <c r="B12" s="33">
         <v>-5.0000000000000001E-3</v>
       </c>
-      <c r="C12" s="35">
+      <c r="C12" s="34">
         <f>D12/(1-$B12)</f>
         <v>53640.65175217107</v>
       </c>
-      <c r="D12" s="35">
+      <c r="D12" s="34">
         <f>E12/(1-$B12)</f>
         <v>53908.855010931919</v>
       </c>
-      <c r="E12" s="36">
+      <c r="E12" s="35">
         <f>D5</f>
         <v>54178.399285986576</v>
       </c>
-      <c r="F12" s="35">
+      <c r="F12" s="34">
         <f>E12</f>
         <v>54178.399285986576</v>
       </c>
-      <c r="G12" s="35">
+      <c r="G12" s="34">
         <f t="shared" ref="G12:AJ12" si="3">F12/(1-$B12)</f>
         <v>53908.855010931919</v>
       </c>
-      <c r="H12" s="35">
+      <c r="H12" s="34">
         <f t="shared" si="3"/>
         <v>53640.65175217107</v>
       </c>
-      <c r="I12" s="35">
+      <c r="I12" s="34">
         <f t="shared" si="3"/>
         <v>53373.782837981169</v>
       </c>
-      <c r="J12" s="35">
+      <c r="J12" s="34">
         <f t="shared" si="3"/>
         <v>53108.241629832017</v>
       </c>
-      <c r="K12" s="35">
+      <c r="K12" s="34">
         <f t="shared" si="3"/>
         <v>52844.021522220915</v>
       </c>
-      <c r="L12" s="35">
+      <c r="L12" s="34">
         <f t="shared" si="3"/>
         <v>52581.115942508382</v>
       </c>
-      <c r="M12" s="35">
+      <c r="M12" s="34">
         <f t="shared" si="3"/>
         <v>52319.518350754617</v>
       </c>
-      <c r="N12" s="35">
+      <c r="N12" s="34">
         <f t="shared" si="3"/>
         <v>52059.222239556839</v>
       </c>
-      <c r="O12" s="35">
+      <c r="O12" s="34">
         <f t="shared" si="3"/>
         <v>51800.221133887404</v>
       </c>
-      <c r="P12" s="35">
+      <c r="P12" s="34">
         <f t="shared" si="3"/>
         <v>51542.508590932746</v>
       </c>
-      <c r="Q12" s="35">
+      <c r="Q12" s="34">
         <f t="shared" si="3"/>
         <v>51286.078199933087</v>
       </c>
-      <c r="R12" s="35">
+      <c r="R12" s="34">
         <f t="shared" si="3"/>
         <v>51030.923582022981</v>
       </c>
-      <c r="S12" s="35">
+      <c r="S12" s="34">
         <f t="shared" si="3"/>
         <v>50777.038390072623</v>
       </c>
-      <c r="T12" s="35">
+      <c r="T12" s="34">
         <f t="shared" si="3"/>
         <v>50524.416308529981</v>
       </c>
-      <c r="U12" s="35">
+      <c r="U12" s="34">
         <f t="shared" si="3"/>
         <v>50273.051053263669</v>
       </c>
-      <c r="V12" s="35">
+      <c r="V12" s="34">
         <f t="shared" si="3"/>
         <v>50022.936371406642</v>
       </c>
-      <c r="W12" s="35">
+      <c r="W12" s="34">
         <f t="shared" si="3"/>
         <v>49774.066041200647</v>
       </c>
-      <c r="X12" s="35">
+      <c r="X12" s="34">
         <f t="shared" si="3"/>
         <v>49526.433871841444</v>
       </c>
-      <c r="Y12" s="35">
+      <c r="Y12" s="34">
         <f t="shared" si="3"/>
         <v>49280.033703324822</v>
       </c>
-      <c r="Z12" s="35">
+      <c r="Z12" s="34">
         <f t="shared" si="3"/>
         <v>49034.859406293363</v>
       </c>
-      <c r="AA12" s="35">
+      <c r="AA12" s="34">
         <f t="shared" si="3"/>
         <v>48790.904881883951</v>
       </c>
-      <c r="AB12" s="35">
+      <c r="AB12" s="34">
         <f t="shared" si="3"/>
         <v>48548.164061576077</v>
       </c>
-      <c r="AC12" s="35">
+      <c r="AC12" s="34">
         <f t="shared" si="3"/>
         <v>48306.630907040875</v>
       </c>
-      <c r="AD12" s="35">
+      <c r="AD12" s="34">
         <f t="shared" si="3"/>
         <v>48066.299409990927</v>
       </c>
-      <c r="AE12" s="35">
+      <c r="AE12" s="34">
         <f t="shared" si="3"/>
         <v>47827.163592030774</v>
       </c>
-      <c r="AF12" s="35">
+      <c r="AF12" s="34">
         <f t="shared" si="3"/>
         <v>47589.21750450824</v>
       </c>
-      <c r="AG12" s="35">
+      <c r="AG12" s="34">
         <f t="shared" si="3"/>
         <v>47352.455228366416</v>
       </c>
-      <c r="AH12" s="35">
+      <c r="AH12" s="34">
         <f t="shared" si="3"/>
         <v>47116.870873996442</v>
       </c>
-      <c r="AI12" s="35">
+      <c r="AI12" s="34">
         <f t="shared" si="3"/>
         <v>46882.458581090992</v>
       </c>
-      <c r="AJ12" s="35">
+      <c r="AJ12" s="34">
         <f t="shared" si="3"/>
         <v>46649.212518498505</v>
       </c>
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A13" s="41" t="s">
+      <c r="A13" s="40" t="s">
         <v>636</v>
       </c>
-      <c r="B13" s="41"/>
-      <c r="C13" s="35">
+      <c r="B13" s="40"/>
+      <c r="C13" s="34">
         <f>C9*1.15</f>
         <v>32913.98254269077</v>
       </c>
-      <c r="D13" s="35">
+      <c r="D13" s="34">
         <f t="shared" ref="D13:AJ13" si="4">D9*1.15</f>
         <v>32912.336925844473</v>
       </c>
-      <c r="E13" s="35">
+      <c r="E13" s="34">
         <f t="shared" si="4"/>
         <v>32910.691391274908</v>
       </c>
-      <c r="F13" s="35">
+      <c r="F13" s="34">
         <f t="shared" si="4"/>
         <v>32909.04593897795</v>
       </c>
-      <c r="G13" s="35">
+      <c r="G13" s="34">
         <f t="shared" si="4"/>
         <v>32907.400568949502</v>
       </c>
-      <c r="H13" s="35">
+      <c r="H13" s="34">
         <f t="shared" si="4"/>
         <v>32905.755281185433</v>
       </c>
-      <c r="I13" s="35">
+      <c r="I13" s="34">
         <f t="shared" si="4"/>
         <v>32904.110075681645</v>
       </c>
-      <c r="J13" s="35">
+      <c r="J13" s="34">
         <f t="shared" si="4"/>
         <v>32902.46495243402</v>
       </c>
-      <c r="K13" s="35">
+      <c r="K13" s="34">
         <f t="shared" si="4"/>
         <v>32900.819911438441</v>
       </c>
-      <c r="L13" s="35">
+      <c r="L13" s="34">
         <f t="shared" si="4"/>
         <v>32899.174952690802</v>
       </c>
-      <c r="M13" s="35">
+      <c r="M13" s="34">
         <f t="shared" si="4"/>
         <v>32897.530076186988</v>
       </c>
-      <c r="N13" s="35">
+      <c r="N13" s="34">
         <f t="shared" si="4"/>
         <v>32895.885281922892</v>
       </c>
-      <c r="O13" s="35">
+      <c r="O13" s="34">
         <f t="shared" si="4"/>
         <v>32894.240569894391</v>
       </c>
-      <c r="P13" s="35">
+      <c r="P13" s="34">
         <f t="shared" si="4"/>
         <v>32892.595940097381</v>
       </c>
-      <c r="Q13" s="35">
+      <c r="Q13" s="34">
         <f t="shared" si="4"/>
         <v>32890.95139252775</v>
       </c>
-      <c r="R13" s="35">
+      <c r="R13" s="34">
         <f t="shared" si="4"/>
         <v>32889.306927181387</v>
       </c>
-      <c r="S13" s="35">
+      <c r="S13" s="34">
         <f t="shared" si="4"/>
         <v>32887.662544054183</v>
       </c>
-      <c r="T13" s="35">
+      <c r="T13" s="34">
         <f t="shared" si="4"/>
         <v>32886.018243142018</v>
       </c>
-      <c r="U13" s="35">
+      <c r="U13" s="34">
         <f t="shared" si="4"/>
         <v>32884.374024440796</v>
       </c>
-      <c r="V13" s="35">
+      <c r="V13" s="34">
         <f t="shared" si="4"/>
         <v>32882.729887946392</v>
       </c>
-      <c r="W13" s="35">
+      <c r="W13" s="34">
         <f t="shared" si="4"/>
         <v>32881.085833654703</v>
       </c>
-      <c r="X13" s="35">
+      <c r="X13" s="34">
         <f t="shared" si="4"/>
         <v>32879.441861561623</v>
       </c>
-      <c r="Y13" s="35">
+      <c r="Y13" s="34">
         <f t="shared" si="4"/>
         <v>32877.797971663036</v>
       </c>
-      <c r="Z13" s="35">
+      <c r="Z13" s="34">
         <f t="shared" si="4"/>
         <v>32876.154163954838</v>
       </c>
-      <c r="AA13" s="35">
+      <c r="AA13" s="34">
         <f t="shared" si="4"/>
         <v>32874.51043843291</v>
       </c>
-      <c r="AB13" s="35">
+      <c r="AB13" s="34">
         <f t="shared" si="4"/>
         <v>32872.866795093149</v>
       </c>
-      <c r="AC13" s="35">
+      <c r="AC13" s="34">
         <f t="shared" si="4"/>
         <v>32871.223233931451</v>
       </c>
-      <c r="AD13" s="35">
+      <c r="AD13" s="34">
         <f t="shared" si="4"/>
         <v>32869.579754943697</v>
       </c>
-      <c r="AE13" s="35">
+      <c r="AE13" s="34">
         <f t="shared" si="4"/>
         <v>32867.936358125786</v>
       </c>
-      <c r="AF13" s="35">
+      <c r="AF13" s="34">
         <f t="shared" si="4"/>
         <v>32866.293043473604</v>
       </c>
-      <c r="AG13" s="35">
+      <c r="AG13" s="34">
         <f t="shared" si="4"/>
         <v>32864.64981098305</v>
       </c>
-      <c r="AH13" s="35">
+      <c r="AH13" s="34">
         <f t="shared" si="4"/>
         <v>32863.006660650019</v>
       </c>
-      <c r="AI13" s="35">
+      <c r="AI13" s="34">
         <f t="shared" si="4"/>
         <v>32861.363592470392</v>
       </c>
-      <c r="AJ13" s="35">
+      <c r="AJ13" s="34">
         <f t="shared" si="4"/>
         <v>32859.720606440067</v>
       </c>
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="40" t="s">
         <v>639</v>
       </c>
-      <c r="B14" s="34">
+      <c r="B14" s="33">
         <v>-5.0000000000000001E-3</v>
       </c>
-      <c r="C14" s="43">
+      <c r="C14" s="42">
         <f>65000*About!$A$144</f>
         <v>79950</v>
       </c>
-      <c r="D14" s="43">
+      <c r="D14" s="42">
         <f>C14/(1-$B14)</f>
         <v>79552.238805970163</v>
       </c>
-      <c r="E14" s="43">
+      <c r="E14" s="42">
         <f t="shared" ref="E14:AJ14" si="5">D14/(1-$B14)</f>
         <v>79156.456523353409</v>
       </c>
-      <c r="F14" s="43">
+      <c r="F14" s="42">
         <f t="shared" si="5"/>
         <v>78762.643306819315</v>
       </c>
-      <c r="G14" s="43">
+      <c r="G14" s="42">
         <f t="shared" si="5"/>
         <v>78370.789360019233</v>
       </c>
-      <c r="H14" s="43">
+      <c r="H14" s="42">
         <f t="shared" si="5"/>
         <v>77980.884935342532</v>
       </c>
-      <c r="I14" s="43">
+      <c r="I14" s="42">
         <f t="shared" si="5"/>
         <v>77592.920333674163</v>
       </c>
-      <c r="J14" s="43">
+      <c r="J14" s="42">
         <f t="shared" si="5"/>
         <v>77206.885904153401</v>
       </c>
-      <c r="K14" s="43">
+      <c r="K14" s="42">
         <f t="shared" si="5"/>
         <v>76822.772043933743</v>
       </c>
-      <c r="L14" s="43">
+      <c r="L14" s="42">
         <f t="shared" si="5"/>
         <v>76440.569197944031</v>
       </c>
-      <c r="M14" s="43">
+      <c r="M14" s="42">
         <f t="shared" si="5"/>
         <v>76060.267858650783</v>
       </c>
-      <c r="N14" s="43">
+      <c r="N14" s="42">
         <f t="shared" si="5"/>
         <v>75681.858565821676</v>
       </c>
-      <c r="O14" s="43">
+      <c r="O14" s="42">
         <f t="shared" si="5"/>
         <v>75305.33190629023</v>
       </c>
-      <c r="P14" s="43">
+      <c r="P14" s="42">
         <f t="shared" si="5"/>
         <v>74930.678513721636</v>
       </c>
-      <c r="Q14" s="43">
+      <c r="Q14" s="42">
         <f t="shared" si="5"/>
         <v>74557.889068379751</v>
       </c>
-      <c r="R14" s="43">
+      <c r="R14" s="42">
         <f t="shared" si="5"/>
         <v>74186.954296895288</v>
       </c>
-      <c r="S14" s="43">
+      <c r="S14" s="42">
         <f t="shared" si="5"/>
         <v>73817.864972035124</v>
       </c>
-      <c r="T14" s="43">
+      <c r="T14" s="42">
         <f t="shared" si="5"/>
         <v>73450.61191247277</v>
       </c>
-      <c r="U14" s="43">
+      <c r="U14" s="42">
         <f t="shared" si="5"/>
         <v>73085.185982559982</v>
       </c>
-      <c r="V14" s="43">
+      <c r="V14" s="42">
         <f t="shared" si="5"/>
         <v>72721.578092099488</v>
       </c>
-      <c r="W14" s="43">
+      <c r="W14" s="42">
         <f t="shared" si="5"/>
         <v>72359.779196118907</v>
       </c>
-      <c r="X14" s="43">
+      <c r="X14" s="42">
         <f t="shared" si="5"/>
         <v>71999.78029464568</v>
       </c>
-      <c r="Y14" s="43">
+      <c r="Y14" s="42">
         <f t="shared" si="5"/>
         <v>71641.57243248327</v>
       </c>
-      <c r="Z14" s="43">
+      <c r="Z14" s="42">
         <f t="shared" si="5"/>
         <v>71285.146698988334</v>
       </c>
-      <c r="AA14" s="43">
+      <c r="AA14" s="42">
         <f t="shared" si="5"/>
         <v>70930.494227849093</v>
       </c>
-      <c r="AB14" s="43">
+      <c r="AB14" s="42">
         <f t="shared" si="5"/>
         <v>70577.60619686477</v>
       </c>
-      <c r="AC14" s="43">
+      <c r="AC14" s="42">
         <f t="shared" si="5"/>
         <v>70226.473827726149</v>
       </c>
-      <c r="AD14" s="43">
+      <c r="AD14" s="42">
         <f t="shared" si="5"/>
         <v>69877.088385797164</v>
       </c>
-      <c r="AE14" s="43">
+      <c r="AE14" s="42">
         <f t="shared" si="5"/>
         <v>69529.44117989768</v>
       </c>
-      <c r="AF14" s="43">
+      <c r="AF14" s="42">
         <f t="shared" si="5"/>
         <v>69183.523562087255</v>
       </c>
-      <c r="AG14" s="43">
+      <c r="AG14" s="42">
         <f t="shared" si="5"/>
         <v>68839.32692745002</v>
       </c>
-      <c r="AH14" s="43">
+      <c r="AH14" s="42">
         <f t="shared" si="5"/>
         <v>68496.842713880629</v>
       </c>
-      <c r="AI14" s="43">
+      <c r="AI14" s="42">
         <f t="shared" si="5"/>
         <v>68156.062401871284</v>
       </c>
-      <c r="AJ14" s="43">
+      <c r="AJ14" s="42">
         <f t="shared" si="5"/>
         <v>67816.977514299797</v>
       </c>
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="40" t="s">
         <v>640</v>
       </c>
-      <c r="B15" s="27"/>
-      <c r="C15" s="43">
+      <c r="B15" s="26"/>
+      <c r="C15" s="42">
         <f>C9*1.05</f>
         <v>30051.897104195923</v>
       </c>
-      <c r="D15" s="43">
+      <c r="D15" s="42">
         <f t="shared" ref="D15:AJ15" si="6">D9*1.05</f>
         <v>30050.394584466696</v>
       </c>
-      <c r="E15" s="43">
+      <c r="E15" s="42">
         <f t="shared" si="6"/>
         <v>30048.892139859701</v>
       </c>
-      <c r="F15" s="43">
+      <c r="F15" s="42">
         <f t="shared" si="6"/>
         <v>30047.389770371177</v>
       </c>
-      <c r="G15" s="43">
+      <c r="G15" s="42">
         <f t="shared" si="6"/>
         <v>30045.887475997373</v>
       </c>
-      <c r="H15" s="43">
+      <c r="H15" s="42">
         <f t="shared" si="6"/>
         <v>30044.385256734531</v>
       </c>
-      <c r="I15" s="43">
+      <c r="I15" s="42">
         <f t="shared" si="6"/>
         <v>30042.883112578897</v>
       </c>
-      <c r="J15" s="43">
+      <c r="J15" s="42">
         <f t="shared" si="6"/>
         <v>30041.381043526715</v>
       </c>
-      <c r="K15" s="43">
+      <c r="K15" s="42">
         <f t="shared" si="6"/>
         <v>30039.879049574232</v>
       </c>
-      <c r="L15" s="43">
+      <c r="L15" s="42">
         <f t="shared" si="6"/>
         <v>30038.377130717694</v>
       </c>
-      <c r="M15" s="43">
+      <c r="M15" s="42">
         <f t="shared" si="6"/>
         <v>30036.875286953342</v>
       </c>
-      <c r="N15" s="43">
+      <c r="N15" s="42">
         <f t="shared" si="6"/>
         <v>30035.373518277425</v>
       </c>
-      <c r="O15" s="43">
+      <c r="O15" s="42">
         <f t="shared" si="6"/>
         <v>30033.871824686186</v>
       </c>
-      <c r="P15" s="43">
+      <c r="P15" s="42">
         <f t="shared" si="6"/>
         <v>30032.370206175874</v>
       </c>
-      <c r="Q15" s="43">
+      <c r="Q15" s="42">
         <f t="shared" si="6"/>
         <v>30030.868662742734</v>
       </c>
-      <c r="R15" s="43">
+      <c r="R15" s="42">
         <f t="shared" si="6"/>
         <v>30029.367194383009</v>
       </c>
-      <c r="S15" s="43">
+      <c r="S15" s="42">
         <f t="shared" si="6"/>
         <v>30027.86580109295</v>
       </c>
-      <c r="T15" s="43">
+      <c r="T15" s="42">
         <f t="shared" si="6"/>
         <v>30026.364482868805</v>
       </c>
-      <c r="U15" s="43">
+      <c r="U15" s="42">
         <f t="shared" si="6"/>
         <v>30024.863239706814</v>
       </c>
-      <c r="V15" s="43">
+      <c r="V15" s="42">
         <f t="shared" si="6"/>
         <v>30023.362071603231</v>
       </c>
-      <c r="W15" s="43">
+      <c r="W15" s="42">
         <f t="shared" si="6"/>
         <v>30021.860978554298</v>
       </c>
-      <c r="X15" s="43">
+      <c r="X15" s="42">
         <f t="shared" si="6"/>
         <v>30020.359960556267</v>
       </c>
-      <c r="Y15" s="43">
+      <c r="Y15" s="42">
         <f t="shared" si="6"/>
         <v>30018.859017605384</v>
       </c>
-      <c r="Z15" s="43">
+      <c r="Z15" s="42">
         <f t="shared" si="6"/>
         <v>30017.358149697895</v>
       </c>
-      <c r="AA15" s="43">
+      <c r="AA15" s="42">
         <f t="shared" si="6"/>
         <v>30015.857356830049</v>
       </c>
-      <c r="AB15" s="43">
+      <c r="AB15" s="42">
         <f t="shared" si="6"/>
         <v>30014.356638998095</v>
       </c>
-      <c r="AC15" s="43">
+      <c r="AC15" s="42">
         <f t="shared" si="6"/>
         <v>30012.855996198283</v>
       </c>
-      <c r="AD15" s="43">
+      <c r="AD15" s="42">
         <f t="shared" si="6"/>
         <v>30011.355428426854</v>
       </c>
-      <c r="AE15" s="43">
+      <c r="AE15" s="42">
         <f t="shared" si="6"/>
         <v>30009.854935680065</v>
       </c>
-      <c r="AF15" s="43">
+      <c r="AF15" s="42">
         <f t="shared" si="6"/>
         <v>30008.354517954162</v>
       </c>
-      <c r="AG15" s="43">
+      <c r="AG15" s="42">
         <f t="shared" si="6"/>
         <v>30006.8541752454</v>
       </c>
-      <c r="AH15" s="43">
+      <c r="AH15" s="42">
         <f t="shared" si="6"/>
         <v>30005.353907550019</v>
       </c>
-      <c r="AI15" s="43">
+      <c r="AI15" s="42">
         <f t="shared" si="6"/>
         <v>30003.853714864272</v>
       </c>
-      <c r="AJ15" s="43">
+      <c r="AJ15" s="42">
         <f t="shared" si="6"/>
         <v>30002.353597184414</v>
       </c>
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A16" s="42"/>
+      <c r="A16" s="41"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -14805,7 +14809,7 @@
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="39" t="s">
+      <c r="A20" s="38" t="s">
         <v>641</v>
       </c>
     </row>
@@ -14828,7 +14832,7 @@
       <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38.140625" customWidth="1"/>
     <col min="2" max="2" width="24.42578125" customWidth="1"/>
@@ -17565,7 +17569,7 @@
   <sheetViews>
     <sheetView topLeftCell="A58" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="69" customWidth="1"/>
     <col min="2" max="2" width="22.85546875" customWidth="1"/>
@@ -19939,7 +19943,7 @@
       <selection activeCell="F5" sqref="F5:F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.140625" customWidth="1"/>
     <col min="2" max="2" width="20.5703125" customWidth="1"/>
@@ -20245,7 +20249,7 @@
       <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="52.140625" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" customWidth="1"/>
@@ -20522,7 +20526,7 @@
       <selection activeCell="B13" sqref="B12:B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.5703125" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
@@ -20611,7 +20615,7 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.42578125" customWidth="1"/>
   </cols>
@@ -21736,7 +21740,7 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.42578125" customWidth="1"/>
     <col min="3" max="4" width="11" bestFit="1" customWidth="1"/>

</xml_diff>